<commit_message>
stubbed in medication related profiles
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-cibmtr-patient.xlsx
+++ b/docs/StructureDefinition-cibmtr-patient.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-02T11:06:34-05:00</t>
+    <t>2022-08-02T15:12:35-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -5547,7 +5547,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
         <v>230</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>85</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>78</v>
@@ -5661,7 +5661,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>230</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>85</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>78</v>
@@ -5775,7 +5775,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
         <v>230</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>85</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>78</v>
@@ -15045,7 +15045,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
         <v>439</v>
       </c>
@@ -15061,7 +15061,7 @@
         <v>77</v>
       </c>
       <c r="G109" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H109" t="s" s="2">
         <v>78</v>
@@ -19381,7 +19381,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
         <v>683</v>
       </c>
@@ -19397,7 +19397,7 @@
         <v>77</v>
       </c>
       <c r="G147" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H147" t="s" s="2">
         <v>78</v>

</xml_diff>